<commit_message>
mengedit dan melengkapi sprint backlog
</commit_message>
<xml_diff>
--- a/PRODUCT_BACKLOG_UTS.xlsx
+++ b/PRODUCT_BACKLOG_UTS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\#AgileDev\UTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="164">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>Anggota yang sudah menyelesaikan task susah dihubungi</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>OPEN</t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,6 +644,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -798,6 +810,15 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,19 +831,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -831,13 +852,13 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1122,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1135,10 +1156,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="2:7" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="B4" s="4" t="s">
@@ -1297,7 +1318,7 @@
         <v>22</v>
       </c>
       <c r="G11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="35.1" customHeight="1">
@@ -1421,16 +1442,16 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="3">
         <f>SUM(G5:G17)</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -1879,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:H157"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1913,10 +1934,10 @@
       </c>
     </row>
     <row r="5" spans="3:8" ht="30" customHeight="1">
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <v>1</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>47</v>
       </c>
       <c r="E5" s="13" t="s">
@@ -1933,8 +1954,8 @@
       </c>
     </row>
     <row r="6" spans="3:8" ht="30" customHeight="1">
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="13" t="s">
         <v>45</v>
       </c>
@@ -1949,8 +1970,8 @@
       </c>
     </row>
     <row r="7" spans="3:8" ht="30" customHeight="1">
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="13" t="s">
         <v>46</v>
       </c>
@@ -1965,10 +1986,10 @@
       </c>
     </row>
     <row r="8" spans="3:8" ht="30" customHeight="1">
-      <c r="C8" s="36">
+      <c r="C8" s="35">
         <v>2</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="35" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="13" t="s">
@@ -1985,8 +2006,8 @@
       </c>
     </row>
     <row r="9" spans="3:8" ht="30" customHeight="1">
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="13" t="s">
         <v>50</v>
       </c>
@@ -2001,8 +2022,8 @@
       </c>
     </row>
     <row r="10" spans="3:8" ht="30" customHeight="1">
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="13" t="s">
         <v>51</v>
       </c>
@@ -2017,8 +2038,8 @@
       </c>
     </row>
     <row r="11" spans="3:8" ht="30" customHeight="1">
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
       <c r="E11" s="13" t="s">
         <v>52</v>
       </c>
@@ -2033,10 +2054,10 @@
       </c>
     </row>
     <row r="12" spans="3:8" ht="45" customHeight="1">
-      <c r="C12" s="35">
+      <c r="C12" s="36">
         <v>3</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="36" t="s">
         <v>58</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -2053,8 +2074,8 @@
       </c>
     </row>
     <row r="13" spans="3:8" ht="35.1" customHeight="1">
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="16" t="s">
         <v>57</v>
       </c>
@@ -2069,10 +2090,10 @@
       </c>
     </row>
     <row r="14" spans="3:8" ht="60" customHeight="1">
-      <c r="C14" s="35">
+      <c r="C14" s="36">
         <v>4</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="36" t="s">
         <v>60</v>
       </c>
       <c r="E14" s="16" t="s">
@@ -2089,8 +2110,8 @@
       </c>
     </row>
     <row r="15" spans="3:8" ht="30" customHeight="1">
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="16" t="s">
         <v>57</v>
       </c>
@@ -2105,10 +2126,10 @@
       </c>
     </row>
     <row r="16" spans="3:8" ht="30" customHeight="1">
-      <c r="C16" s="35">
+      <c r="C16" s="36">
         <v>5</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="36" t="s">
         <v>64</v>
       </c>
       <c r="E16" s="16" t="s">
@@ -2125,8 +2146,8 @@
       </c>
     </row>
     <row r="17" spans="3:8" ht="30" customHeight="1">
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="16" t="s">
         <v>62</v>
       </c>
@@ -2141,8 +2162,8 @@
       </c>
     </row>
     <row r="18" spans="3:8" ht="30" customHeight="1">
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="16" t="s">
         <v>63</v>
       </c>
@@ -2157,56 +2178,62 @@
       </c>
     </row>
     <row r="19" spans="3:8" ht="30" customHeight="1">
-      <c r="C19" s="34">
-        <v>6</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="C19" s="37">
+        <v>9</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="8">
-        <v>1</v>
-      </c>
-      <c r="H19" s="8"/>
+      <c r="G19" s="28">
+        <v>2</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="20" spans="3:8" ht="30" customHeight="1">
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="28">
         <v>2</v>
       </c>
-      <c r="H20" s="8"/>
+      <c r="H20" s="28" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="21" spans="3:8" ht="30" customHeight="1">
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="8" t="s">
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="28">
         <v>3</v>
       </c>
-      <c r="H21" s="8"/>
+      <c r="H21" s="28" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="22" spans="3:8" ht="46.5" customHeight="1">
-      <c r="C22" s="34">
+      <c r="C22" s="37">
         <v>7</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="37" t="s">
         <v>72</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -2218,11 +2245,13 @@
       <c r="G22" s="8">
         <v>1</v>
       </c>
-      <c r="H22" s="8"/>
+      <c r="H22" s="8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="23" spans="3:8" ht="30" customHeight="1">
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="8" t="s">
         <v>69</v>
       </c>
@@ -2232,11 +2261,13 @@
       <c r="G23" s="8">
         <v>1</v>
       </c>
-      <c r="H23" s="8"/>
+      <c r="H23" s="8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="24" spans="3:8" ht="30" customHeight="1">
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="8" t="s">
         <v>70</v>
       </c>
@@ -2246,11 +2277,13 @@
       <c r="G24" s="8">
         <v>2</v>
       </c>
-      <c r="H24" s="8"/>
+      <c r="H24" s="8" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="25" spans="3:8" ht="45">
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="8" t="s">
         <v>71</v>
       </c>
@@ -2260,13 +2293,15 @@
       <c r="G25" s="8">
         <v>3</v>
       </c>
-      <c r="H25" s="8"/>
+      <c r="H25" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="26" spans="3:8" ht="45" customHeight="1">
-      <c r="C26" s="34">
+      <c r="C26" s="37">
         <v>8</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="37" t="s">
         <v>73</v>
       </c>
       <c r="E26" s="8" t="s">
@@ -2278,11 +2313,13 @@
       <c r="G26" s="8">
         <v>1</v>
       </c>
-      <c r="H26" s="8"/>
+      <c r="H26" s="8" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="27" spans="3:8" ht="45" customHeight="1">
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="8" t="s">
         <v>75</v>
       </c>
@@ -2292,65 +2329,67 @@
       <c r="G27" s="8">
         <v>3</v>
       </c>
-      <c r="H27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="28" spans="3:8" ht="35.1" customHeight="1">
-      <c r="C28" s="33">
-        <v>9</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="12" t="s">
+      <c r="C28" s="43">
+        <v>6</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="44">
+        <v>1</v>
+      </c>
+      <c r="H28" s="44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" ht="35.1" customHeight="1">
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="44">
         <v>2</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H29" s="44" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="3:8" ht="35.1" customHeight="1">
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F29" s="12" t="s">
+    <row r="30" spans="3:8" ht="35.1" customHeight="1">
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="12">
-        <v>2</v>
-      </c>
-      <c r="H29" s="19" t="s">
+      <c r="G30" s="44">
+        <v>3</v>
+      </c>
+      <c r="H30" s="44" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="3:8" ht="35.1" customHeight="1">
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="12">
-        <v>3</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
     <row r="31" spans="3:8" ht="30" customHeight="1">
-      <c r="C31" s="33">
+      <c r="C31" s="38">
         <v>10</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="38" t="s">
         <v>82</v>
       </c>
       <c r="E31" s="12" t="s">
@@ -2367,8 +2406,8 @@
       </c>
     </row>
     <row r="32" spans="3:8" ht="30" customHeight="1">
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="12" t="s">
         <v>80</v>
       </c>
@@ -2383,8 +2422,8 @@
       </c>
     </row>
     <row r="33" spans="3:8" ht="30" customHeight="1">
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
       <c r="E33" s="12" t="s">
         <v>81</v>
       </c>
@@ -2399,8 +2438,8 @@
       </c>
     </row>
     <row r="34" spans="3:8" ht="30" customHeight="1">
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
       <c r="E34" s="12" t="s">
         <v>57</v>
       </c>
@@ -2415,10 +2454,10 @@
       </c>
     </row>
     <row r="35" spans="3:8" ht="45" customHeight="1">
-      <c r="C35" s="33">
+      <c r="C35" s="38">
         <v>11</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="38" t="s">
         <v>85</v>
       </c>
       <c r="E35" s="12" t="s">
@@ -2435,8 +2474,8 @@
       </c>
     </row>
     <row r="36" spans="3:8" ht="45" customHeight="1">
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
       <c r="E36" s="12" t="s">
         <v>84</v>
       </c>
@@ -2451,10 +2490,10 @@
       </c>
     </row>
     <row r="37" spans="3:8" ht="30" customHeight="1">
-      <c r="C37" s="32">
+      <c r="C37" s="39">
         <v>12</v>
       </c>
-      <c r="D37" s="32" t="s">
+      <c r="D37" s="39" t="s">
         <v>86</v>
       </c>
       <c r="E37" s="15" t="s">
@@ -2471,8 +2510,8 @@
       </c>
     </row>
     <row r="38" spans="3:8" ht="30" customHeight="1">
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
       <c r="E38" s="15" t="s">
         <v>88</v>
       </c>
@@ -2487,8 +2526,8 @@
       </c>
     </row>
     <row r="39" spans="3:8" ht="30" customHeight="1">
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
       <c r="E39" s="15" t="s">
         <v>89</v>
       </c>
@@ -2503,8 +2542,8 @@
       </c>
     </row>
     <row r="40" spans="3:8" ht="30" customHeight="1">
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
       <c r="E40" s="15" t="s">
         <v>90</v>
       </c>
@@ -2519,8 +2558,8 @@
       </c>
     </row>
     <row r="41" spans="3:8" ht="30" customHeight="1">
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
       <c r="E41" s="15" t="s">
         <v>91</v>
       </c>
@@ -2535,8 +2574,8 @@
       </c>
     </row>
     <row r="42" spans="3:8" ht="30" customHeight="1">
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
       <c r="E42" s="15" t="s">
         <v>57</v>
       </c>
@@ -2551,10 +2590,10 @@
       </c>
     </row>
     <row r="43" spans="3:8" ht="30" customHeight="1">
-      <c r="C43" s="32">
+      <c r="C43" s="39">
         <v>13</v>
       </c>
-      <c r="D43" s="32" t="s">
+      <c r="D43" s="39" t="s">
         <v>94</v>
       </c>
       <c r="E43" s="15" t="s">
@@ -2571,8 +2610,8 @@
       </c>
     </row>
     <row r="44" spans="3:8" ht="30" customHeight="1">
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
       <c r="E44" s="15" t="s">
         <v>93</v>
       </c>
@@ -2587,8 +2626,8 @@
       </c>
     </row>
     <row r="45" spans="3:8" ht="30" customHeight="1">
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
       <c r="E45" s="15" t="s">
         <v>57</v>
       </c>
@@ -3500,24 +3539,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="C28:C30"/>
     <mergeCell ref="D43:D45"/>
     <mergeCell ref="C43:C45"/>
     <mergeCell ref="D31:D34"/>
@@ -3526,6 +3547,24 @@
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D37:D42"/>
     <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3547,10 +3586,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" s="21" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="41"/>
     </row>
     <row r="6" spans="2:5" s="21" customFormat="1" ht="30" customHeight="1">
       <c r="B6" s="22" t="s">
@@ -3633,10 +3672,10 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.899999999999999" customHeight="1">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="38"/>
+      <c r="C17" s="41"/>
     </row>
     <row r="18" spans="2:8" ht="30" customHeight="1">
       <c r="B18" s="22" t="s">
@@ -3722,10 +3761,10 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="38"/>
+      <c r="C29" s="41"/>
     </row>
     <row r="30" spans="2:8" ht="34.9" customHeight="1">
       <c r="B30" s="22" t="s">
@@ -3811,10 +3850,10 @@
       </c>
     </row>
     <row r="41" spans="2:6" ht="19.899999999999999" customHeight="1">
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="37"/>
+      <c r="C41" s="40"/>
     </row>
     <row r="42" spans="2:6" ht="34.9" customHeight="1">
       <c r="B42" s="22" t="s">
@@ -3897,10 +3936,10 @@
       </c>
     </row>
     <row r="53" spans="2:5" ht="19.899999999999999" customHeight="1">
-      <c r="B53" s="37" t="s">
+      <c r="B53" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C53" s="37"/>
+      <c r="C53" s="40"/>
     </row>
     <row r="54" spans="2:5" ht="34.9" customHeight="1">
       <c r="B54" s="22" t="s">
@@ -3983,10 +4022,10 @@
       </c>
     </row>
     <row r="65" spans="2:5" ht="19.899999999999999" customHeight="1">
-      <c r="B65" s="37" t="s">
+      <c r="B65" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="37"/>
+      <c r="C65" s="40"/>
     </row>
     <row r="66" spans="2:5" ht="34.9" customHeight="1">
       <c r="B66" s="22" t="s">
@@ -4086,7 +4125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4094,25 +4133,25 @@
   <cols>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:4" ht="30" customHeight="1">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="30" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="45" customHeight="1">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>150</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -4120,38 +4159,38 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="45" customHeight="1">
-      <c r="B8" s="40"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="17" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="45" customHeight="1">
-      <c r="B9" s="40"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="17" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="45" customHeight="1">
-      <c r="B10" s="40"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="45" customHeight="1">
-      <c r="B11" s="40"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="17" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="36" t="s">
         <v>156</v>
       </c>
       <c r="D12" s="18" t="s">
@@ -4159,36 +4198,36 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="18" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="18" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="18" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="18" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="18" t="s">
         <v>161</v>
       </c>

</xml_diff>

<commit_message>
edit sprint backlog dan retrospective
</commit_message>
<xml_diff>
--- a/PRODUCT_BACKLOG_UTS.xlsx
+++ b/PRODUCT_BACKLOG_UTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7710" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7710" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="165">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -506,18 +506,12 @@
     <t>pengerjaan task yang jauh lewat dari estimasi</t>
   </si>
   <si>
-    <t>Pada sprint 2 dengan goals “user bisa membuat catatan transaksi”. Kelompok kami terlah berhasil mengembangkan fitur “tambah transaksi” dimana nantinya user bisa menginput pengeluaran dan pendapatan dengan meyertakan detail seperti kategori, rekening yang digunakan, nominal, catatan, dan waktu. Yang kemudian catatan transaksi yang di input dapat tampil dan di lihat di menu transaksi. Setelah demo, semua anggota puas dengan fitur utama dari aplikasi ini karena berhasil mengimplementasikan fitur utama dari aplikasi persis seperti yang direncakan di awal. Adapun fitur lain yang berhasil dikembangkan adalah fitur “tambah rekening” yang berjalan cukup lancar</t>
-  </si>
-  <si>
     <t>Sebagai user, saya ingin bisa membuat catatan transaksi</t>
   </si>
   <si>
     <t>Pengerjaan task yang on time</t>
   </si>
   <si>
-    <t>Diskusi antar sesama anggota dalam memecahkanmasalah yang berjalan secara kondusif</t>
-  </si>
-  <si>
     <t>Daily SCRUM meeting tidak tepat waktu</t>
   </si>
   <si>
@@ -528,6 +522,15 @@
   </si>
   <si>
     <t>OPEN</t>
+  </si>
+  <si>
+    <t>design awal yang kurang memenuhi ekspektasi</t>
+  </si>
+  <si>
+    <t>Pada sprint 2 dengan goals “user bisa membuat catatan transaksi”. Kelompok kami terlah berhasil mengembangkan fitur “tambah transaksi” dimana nantinya user bisa menginput pengeluaran dan pendapatan dengan meyertakan detail seperti kategori, rekening yang digunakan, nominal, catatan, dan waktu. Yang kemudian catatan transaksi yang di input dapat tampil dan di lihat di menu transaksi. Setelah demo, semua anggota puas dengan fitur utama dari aplikasi ini karena berhasil mengimplementasikan fitur utama dari aplikasi persis seperti yang direncakan di awal. Adapun fitur lain yang berhasil dikembangkan adalah fitur “tambah rekening” yang berhasil di selesaikan dengan lancar</t>
+  </si>
+  <si>
+    <t>Diskusi antar sesama anggota dalam memecahkan masalah yang berjalan secara kondusif</t>
   </si>
 </sst>
 </file>
@@ -727,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -819,6 +822,12 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -831,19 +840,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,12 +865,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1156,10 +1162,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="33"/>
     </row>
     <row r="4" spans="2:7" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="B4" s="4" t="s">
@@ -1442,13 +1448,13 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="3">
         <f>SUM(G5:G17)</f>
         <v>41</v>
@@ -1900,7 +1906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:H157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -1934,10 +1940,10 @@
       </c>
     </row>
     <row r="5" spans="3:8" ht="30" customHeight="1">
-      <c r="C5" s="35">
+      <c r="C5" s="42">
         <v>1</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="42" t="s">
         <v>47</v>
       </c>
       <c r="E5" s="13" t="s">
@@ -1954,8 +1960,8 @@
       </c>
     </row>
     <row r="6" spans="3:8" ht="30" customHeight="1">
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
       <c r="E6" s="13" t="s">
         <v>45</v>
       </c>
@@ -1970,8 +1976,8 @@
       </c>
     </row>
     <row r="7" spans="3:8" ht="30" customHeight="1">
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="13" t="s">
         <v>46</v>
       </c>
@@ -1986,10 +1992,10 @@
       </c>
     </row>
     <row r="8" spans="3:8" ht="30" customHeight="1">
-      <c r="C8" s="35">
+      <c r="C8" s="42">
         <v>2</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="42" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="13" t="s">
@@ -2006,8 +2012,8 @@
       </c>
     </row>
     <row r="9" spans="3:8" ht="30" customHeight="1">
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="13" t="s">
         <v>50</v>
       </c>
@@ -2022,8 +2028,8 @@
       </c>
     </row>
     <row r="10" spans="3:8" ht="30" customHeight="1">
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="13" t="s">
         <v>51</v>
       </c>
@@ -2038,8 +2044,8 @@
       </c>
     </row>
     <row r="11" spans="3:8" ht="30" customHeight="1">
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
       <c r="E11" s="13" t="s">
         <v>52</v>
       </c>
@@ -2054,10 +2060,10 @@
       </c>
     </row>
     <row r="12" spans="3:8" ht="45" customHeight="1">
-      <c r="C12" s="36">
+      <c r="C12" s="40">
         <v>3</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="40" t="s">
         <v>58</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -2074,8 +2080,8 @@
       </c>
     </row>
     <row r="13" spans="3:8" ht="35.1" customHeight="1">
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="16" t="s">
         <v>57</v>
       </c>
@@ -2090,10 +2096,10 @@
       </c>
     </row>
     <row r="14" spans="3:8" ht="60" customHeight="1">
-      <c r="C14" s="36">
+      <c r="C14" s="40">
         <v>4</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="40" t="s">
         <v>60</v>
       </c>
       <c r="E14" s="16" t="s">
@@ -2110,8 +2116,8 @@
       </c>
     </row>
     <row r="15" spans="3:8" ht="30" customHeight="1">
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
       <c r="E15" s="16" t="s">
         <v>57</v>
       </c>
@@ -2126,10 +2132,10 @@
       </c>
     </row>
     <row r="16" spans="3:8" ht="30" customHeight="1">
-      <c r="C16" s="36">
+      <c r="C16" s="40">
         <v>5</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="40" t="s">
         <v>64</v>
       </c>
       <c r="E16" s="16" t="s">
@@ -2146,8 +2152,8 @@
       </c>
     </row>
     <row r="17" spans="3:8" ht="30" customHeight="1">
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="16" t="s">
         <v>62</v>
       </c>
@@ -2162,8 +2168,8 @@
       </c>
     </row>
     <row r="18" spans="3:8" ht="30" customHeight="1">
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="16" t="s">
         <v>63</v>
       </c>
@@ -2178,10 +2184,10 @@
       </c>
     </row>
     <row r="19" spans="3:8" ht="30" customHeight="1">
-      <c r="C19" s="37">
+      <c r="C19" s="39">
         <v>9</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="39" t="s">
         <v>78</v>
       </c>
       <c r="E19" s="28" t="s">
@@ -2194,12 +2200,12 @@
         <v>2</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="30" customHeight="1">
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
       <c r="E20" s="28" t="s">
         <v>77</v>
       </c>
@@ -2210,12 +2216,12 @@
         <v>2</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="30" customHeight="1">
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
       <c r="E21" s="28" t="s">
         <v>57</v>
       </c>
@@ -2226,14 +2232,14 @@
         <v>3</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="46.5" customHeight="1">
-      <c r="C22" s="37">
+      <c r="C22" s="39">
         <v>7</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="39" t="s">
         <v>72</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -2250,8 +2256,8 @@
       </c>
     </row>
     <row r="23" spans="3:8" ht="30" customHeight="1">
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
       <c r="E23" s="8" t="s">
         <v>69</v>
       </c>
@@ -2266,8 +2272,8 @@
       </c>
     </row>
     <row r="24" spans="3:8" ht="30" customHeight="1">
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
       <c r="E24" s="8" t="s">
         <v>70</v>
       </c>
@@ -2278,12 +2284,12 @@
         <v>2</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="45">
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="8" t="s">
         <v>71</v>
       </c>
@@ -2298,10 +2304,10 @@
       </c>
     </row>
     <row r="26" spans="3:8" ht="45" customHeight="1">
-      <c r="C26" s="37">
+      <c r="C26" s="39">
         <v>8</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="39" t="s">
         <v>73</v>
       </c>
       <c r="E26" s="8" t="s">
@@ -2314,12 +2320,12 @@
         <v>1</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="45" customHeight="1">
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
       <c r="E27" s="8" t="s">
         <v>75</v>
       </c>
@@ -2334,54 +2340,54 @@
       </c>
     </row>
     <row r="28" spans="3:8" ht="35.1" customHeight="1">
-      <c r="C28" s="43">
+      <c r="C28" s="41">
         <v>6</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="44" t="s">
+      <c r="E28" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="44" t="s">
+      <c r="F28" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="44">
+      <c r="G28" s="32">
         <v>1</v>
       </c>
-      <c r="H28" s="44" t="s">
+      <c r="H28" s="32" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="35.1" customHeight="1">
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="44" t="s">
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="44" t="s">
+      <c r="F29" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="44">
+      <c r="G29" s="32">
         <v>2</v>
       </c>
-      <c r="H29" s="44" t="s">
+      <c r="H29" s="32" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="35.1" customHeight="1">
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="44" t="s">
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="44" t="s">
+      <c r="F30" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="44">
+      <c r="G30" s="32">
         <v>3</v>
       </c>
-      <c r="H30" s="44" t="s">
+      <c r="H30" s="32" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2490,10 +2496,10 @@
       </c>
     </row>
     <row r="37" spans="3:8" ht="30" customHeight="1">
-      <c r="C37" s="39">
+      <c r="C37" s="37">
         <v>12</v>
       </c>
-      <c r="D37" s="39" t="s">
+      <c r="D37" s="37" t="s">
         <v>86</v>
       </c>
       <c r="E37" s="15" t="s">
@@ -2510,8 +2516,8 @@
       </c>
     </row>
     <row r="38" spans="3:8" ht="30" customHeight="1">
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="15" t="s">
         <v>88</v>
       </c>
@@ -2526,8 +2532,8 @@
       </c>
     </row>
     <row r="39" spans="3:8" ht="30" customHeight="1">
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="15" t="s">
         <v>89</v>
       </c>
@@ -2542,8 +2548,8 @@
       </c>
     </row>
     <row r="40" spans="3:8" ht="30" customHeight="1">
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="15" t="s">
         <v>90</v>
       </c>
@@ -2558,8 +2564,8 @@
       </c>
     </row>
     <row r="41" spans="3:8" ht="30" customHeight="1">
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="15" t="s">
         <v>91</v>
       </c>
@@ -2574,8 +2580,8 @@
       </c>
     </row>
     <row r="42" spans="3:8" ht="30" customHeight="1">
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
       <c r="E42" s="15" t="s">
         <v>57</v>
       </c>
@@ -2590,10 +2596,10 @@
       </c>
     </row>
     <row r="43" spans="3:8" ht="30" customHeight="1">
-      <c r="C43" s="39">
+      <c r="C43" s="37">
         <v>13</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="37" t="s">
         <v>94</v>
       </c>
       <c r="E43" s="15" t="s">
@@ -2610,8 +2616,8 @@
       </c>
     </row>
     <row r="44" spans="3:8" ht="30" customHeight="1">
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="15" t="s">
         <v>93</v>
       </c>
@@ -2626,8 +2632,8 @@
       </c>
     </row>
     <row r="45" spans="3:8" ht="30" customHeight="1">
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="15" t="s">
         <v>57</v>
       </c>
@@ -3539,6 +3545,24 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="C19:C21"/>
     <mergeCell ref="D43:D45"/>
     <mergeCell ref="C43:C45"/>
     <mergeCell ref="D31:D34"/>
@@ -3547,24 +3571,6 @@
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D37:D42"/>
     <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3574,7 +3580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="94" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="94" workbookViewId="0">
       <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
@@ -3586,10 +3592,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" s="21" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="44"/>
     </row>
     <row r="6" spans="2:5" s="21" customFormat="1" ht="30" customHeight="1">
       <c r="B6" s="22" t="s">
@@ -3672,10 +3678,10 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.899999999999999" customHeight="1">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="41"/>
+      <c r="C17" s="44"/>
     </row>
     <row r="18" spans="2:8" ht="30" customHeight="1">
       <c r="B18" s="22" t="s">
@@ -3761,10 +3767,10 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="19.899999999999999" customHeight="1">
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="41"/>
+      <c r="C29" s="44"/>
     </row>
     <row r="30" spans="2:8" ht="34.9" customHeight="1">
       <c r="B30" s="22" t="s">
@@ -3850,10 +3856,10 @@
       </c>
     </row>
     <row r="41" spans="2:6" ht="19.899999999999999" customHeight="1">
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="40"/>
+      <c r="C41" s="43"/>
     </row>
     <row r="42" spans="2:6" ht="34.9" customHeight="1">
       <c r="B42" s="22" t="s">
@@ -3936,10 +3942,10 @@
       </c>
     </row>
     <row r="53" spans="2:5" ht="19.899999999999999" customHeight="1">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="43"/>
     </row>
     <row r="54" spans="2:5" ht="34.9" customHeight="1">
       <c r="B54" s="22" t="s">
@@ -4022,10 +4028,10 @@
       </c>
     </row>
     <row r="65" spans="2:5" ht="19.899999999999999" customHeight="1">
-      <c r="B65" s="40" t="s">
+      <c r="B65" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="40"/>
+      <c r="C65" s="43"/>
     </row>
     <row r="66" spans="2:5" ht="34.9" customHeight="1">
       <c r="B66" s="22" t="s">
@@ -4123,10 +4129,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:D50"/>
+  <dimension ref="B6:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4148,10 +4154,10 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="45" customHeight="1">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="42" t="s">
         <v>150</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -4159,83 +4165,85 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="45" customHeight="1">
-      <c r="B8" s="42"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="17" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="45" customHeight="1">
-      <c r="B9" s="42"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="17" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="45" customHeight="1">
-      <c r="B10" s="42"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="45" customHeight="1">
-      <c r="B11" s="42"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="17" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="31" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="45" customHeight="1">
+      <c r="B12" s="45"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B12" s="36" t="s">
+    <row r="13" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B13" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="18" t="s">
+    </row>
+    <row r="15" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="18" t="s">
+    <row r="18" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="18" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="2"/>
@@ -4397,12 +4405,17 @@
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="B13:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>